<commit_message>
distinct result figures added
</commit_message>
<xml_diff>
--- a/EJBComponents/ImageProcessingBenchmark/stats/OverallRuntimes.xlsx
+++ b/EJBComponents/ImageProcessingBenchmark/stats/OverallRuntimes.xlsx
@@ -188,30 +188,30 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -263,7 +263,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-NZ"/>
+              <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
               <a:t>Overall Runtimes</a:t>
             </a:r>
           </a:p>
@@ -306,10 +306,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.7235062707230874E-2"/>
-          <c:y val="7.0871794733189775E-2"/>
-          <c:w val="0.9217172507016298"/>
-          <c:h val="0.85448938374144479"/>
+          <c:x val="9.2254068241469811E-2"/>
+          <c:y val="6.2941227804644187E-2"/>
+          <c:w val="0.88669816272965885"/>
+          <c:h val="0.84061088775490933"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -319,7 +319,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Local-ResourceContention</c:v>
+            <c:v>Proportional Allocation - Local</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -421,7 +421,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Remote-ResourceContention</c:v>
+            <c:v>Proportional Allocation - Remote</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -523,7 +523,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Local-FourThreads</c:v>
+            <c:v>Partial Allocation - Local</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -629,7 +629,7 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Remote-FourThreads</c:v>
+            <c:v>Partial Allocation - Remote</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -735,7 +735,7 @@
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Local-EightHyperThreads</c:v>
+            <c:v>Full Allocation - Local</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -837,7 +837,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Remote-EightHyperThreads</c:v>
+            <c:v>Full Allocation - Remote</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="15875" cap="rnd">
@@ -945,11 +945,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1128410448"/>
-        <c:axId val="1128410992"/>
+        <c:axId val="396772672"/>
+        <c:axId val="396773760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1128410448"/>
+        <c:axId val="396772672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,7 +989,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ"/>
+                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
                   <a:t>Number of Sub-Images</a:t>
                 </a:r>
               </a:p>
@@ -999,8 +999,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.44163869239208836"/>
-              <c:y val="0.95796673799804988"/>
+              <c:x val="0.40704410867560475"/>
+              <c:y val="0.95533085850533361"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1051,7 +1051,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:ln>
                   <a:noFill/>
                 </a:ln>
@@ -1069,7 +1069,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1128410992"/>
+        <c:crossAx val="396773760"/>
         <c:crossesAt val="0"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -1077,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1128410992"/>
+        <c:axId val="396773760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="55"/>
@@ -1132,8 +1132,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-NZ"/>
-                  <a:t>Time in Minutes</a:t>
+                  <a:rPr lang="en-NZ" sz="1600" baseline="0"/>
+                  <a:t>Time (Minutes)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1142,8 +1142,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="6.1585835257890681E-3"/>
-              <c:y val="0.41934896992932857"/>
+              <c:x val="1.8342626090657587E-3"/>
+              <c:y val="0.36779998885343879"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1193,7 +1193,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1208,7 +1208,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1128410448"/>
+        <c:crossAx val="396772672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
@@ -1224,7 +1224,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.709562828970703"/>
+          <c:y val="6.6478309556864873E-2"/>
+          <c:w val="0.28034708093920691"/>
+          <c:h val="0.20074488378304919"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1238,7 +1247,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1836,15 +1845,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2155,8 +2164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G43" workbookViewId="0">
-      <selection activeCell="Z60" sqref="Z60"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2167,1524 +2176,1524 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>6</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>8</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>10</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>12</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>14</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>36</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>20.5</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>17.5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>12.5</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>14.5</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>15</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>17</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>12</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>26</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>13.5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>8.5</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>10</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>8.5</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>8</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>8</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>6</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <v>8</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>10</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>12</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>14</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>30</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>18.5</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>15</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>12.5</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>18</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>20</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>19</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>19</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <v>18.5</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>26</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>13.5</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>9.5</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>11</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>10</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>10.5</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>10</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>10.5</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>6</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="2">
         <v>8</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>10</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>12</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>14</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>54.5</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>23.5</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>22</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>16</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>16.5</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>16.5</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>17</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>17</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>26</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>13.5</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>10</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>9</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>9</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>8</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>8</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>10</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="L26" s="8" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="L26" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="T26" s="8"/>
-      <c r="U26" s="8"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="L27" s="1" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="L27" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1"/>
-      <c r="S27" s="1"/>
-      <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="7">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>2</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>4</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>6</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="4">
         <v>8</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>10</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="4">
         <v>12</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="4">
         <v>14</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="4">
         <v>16</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="4">
         <v>1</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="4">
         <v>2</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="4">
         <v>4</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="4">
         <v>6</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="4">
         <v>8</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R28" s="4">
         <v>10</v>
       </c>
-      <c r="S28" s="7">
+      <c r="S28" s="4">
         <v>12</v>
       </c>
-      <c r="T28" s="7">
+      <c r="T28" s="4">
         <v>14</v>
       </c>
-      <c r="U28" s="7">
+      <c r="U28" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="M29" s="6" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="M29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="6"/>
-      <c r="T29" s="6"/>
-      <c r="U29" s="6"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>70979</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>48338</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>28628</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>24985</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>22166</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>29680</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>26513</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>25838</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>26814</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="L30" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="9">
+      <c r="M30" s="5">
         <f>B30/1000</f>
         <v>70.978999999999999</v>
       </c>
-      <c r="N30" s="9">
+      <c r="N30" s="5">
         <f t="shared" ref="N30:U30" si="0">C30/1000</f>
         <v>48.338000000000001</v>
       </c>
-      <c r="O30" s="9">
+      <c r="O30" s="5">
         <f t="shared" si="0"/>
         <v>28.628</v>
       </c>
-      <c r="P30" s="9">
+      <c r="P30" s="5">
         <f t="shared" si="0"/>
         <v>24.984999999999999</v>
       </c>
-      <c r="Q30" s="9">
+      <c r="Q30" s="5">
         <f t="shared" si="0"/>
         <v>22.166</v>
       </c>
-      <c r="R30" s="9">
+      <c r="R30" s="5">
         <f t="shared" si="0"/>
         <v>29.68</v>
       </c>
-      <c r="S30" s="9">
+      <c r="S30" s="5">
         <f t="shared" si="0"/>
         <v>26.513000000000002</v>
       </c>
-      <c r="T30" s="9">
+      <c r="T30" s="5">
         <f t="shared" si="0"/>
         <v>25.838000000000001</v>
       </c>
-      <c r="U30" s="9">
+      <c r="U30" s="5">
         <f t="shared" si="0"/>
         <v>26.814</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>98836</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>59284</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>42700</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>50867</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>45531</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>50644</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="1">
         <v>46199</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>51517</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
         <v>55666</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="L31" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="9">
+      <c r="M31" s="5">
         <f t="shared" ref="M31:M34" si="1">B31/1000</f>
         <v>98.835999999999999</v>
       </c>
-      <c r="N31" s="9">
+      <c r="N31" s="5">
         <f t="shared" ref="N31:N34" si="2">C31/1000</f>
         <v>59.283999999999999</v>
       </c>
-      <c r="O31" s="9">
+      <c r="O31" s="5">
         <f t="shared" ref="O31:O34" si="3">D31/1000</f>
         <v>42.7</v>
       </c>
-      <c r="P31" s="9">
+      <c r="P31" s="5">
         <f t="shared" ref="P31:P34" si="4">E31/1000</f>
         <v>50.866999999999997</v>
       </c>
-      <c r="Q31" s="9">
+      <c r="Q31" s="5">
         <f t="shared" ref="Q31:Q34" si="5">F31/1000</f>
         <v>45.530999999999999</v>
       </c>
-      <c r="R31" s="9">
+      <c r="R31" s="5">
         <f t="shared" ref="R31:R34" si="6">G31/1000</f>
         <v>50.643999999999998</v>
       </c>
-      <c r="S31" s="9">
+      <c r="S31" s="5">
         <f t="shared" ref="S31:S34" si="7">H31/1000</f>
         <v>46.198999999999998</v>
       </c>
-      <c r="T31" s="9">
+      <c r="T31" s="5">
         <f t="shared" ref="T31:T34" si="8">I31/1000</f>
         <v>51.517000000000003</v>
       </c>
-      <c r="U31" s="9">
+      <c r="U31" s="5">
         <f t="shared" ref="U31:U34" si="9">J31/1000</f>
         <v>55.665999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>104548</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>63684</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>50097</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>58621</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>58532</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>65473</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>79563</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>71250</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>94615</v>
       </c>
-      <c r="L32" s="2" t="s">
+      <c r="L32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M32" s="9">
+      <c r="M32" s="5">
         <f t="shared" si="1"/>
         <v>104.548</v>
       </c>
-      <c r="N32" s="9">
+      <c r="N32" s="5">
         <f t="shared" si="2"/>
         <v>63.683999999999997</v>
       </c>
-      <c r="O32" s="9">
+      <c r="O32" s="5">
         <f t="shared" si="3"/>
         <v>50.097000000000001</v>
       </c>
-      <c r="P32" s="9">
+      <c r="P32" s="5">
         <f t="shared" si="4"/>
         <v>58.621000000000002</v>
       </c>
-      <c r="Q32" s="9">
+      <c r="Q32" s="5">
         <f t="shared" si="5"/>
         <v>58.531999999999996</v>
       </c>
-      <c r="R32" s="9">
+      <c r="R32" s="5">
         <f t="shared" si="6"/>
         <v>65.472999999999999</v>
       </c>
-      <c r="S32" s="9">
+      <c r="S32" s="5">
         <f t="shared" si="7"/>
         <v>79.563000000000002</v>
       </c>
-      <c r="T32" s="9">
+      <c r="T32" s="5">
         <f t="shared" si="8"/>
         <v>71.25</v>
       </c>
-      <c r="U32" s="9">
+      <c r="U32" s="5">
         <f t="shared" si="9"/>
         <v>94.614999999999995</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>292674</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>173329</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>178082</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>124792</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>108968</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>136526</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>142538</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <v>113560</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>125407</v>
       </c>
-      <c r="L33" s="2" t="s">
+      <c r="L33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M33" s="9">
+      <c r="M33" s="5">
         <f t="shared" si="1"/>
         <v>292.67399999999998</v>
       </c>
-      <c r="N33" s="9">
+      <c r="N33" s="5">
         <f t="shared" si="2"/>
         <v>173.32900000000001</v>
       </c>
-      <c r="O33" s="9">
+      <c r="O33" s="5">
         <f t="shared" si="3"/>
         <v>178.08199999999999</v>
       </c>
-      <c r="P33" s="9">
+      <c r="P33" s="5">
         <f t="shared" si="4"/>
         <v>124.792</v>
       </c>
-      <c r="Q33" s="9">
+      <c r="Q33" s="5">
         <f t="shared" si="5"/>
         <v>108.968</v>
       </c>
-      <c r="R33" s="9">
+      <c r="R33" s="5">
         <f t="shared" si="6"/>
         <v>136.52600000000001</v>
       </c>
-      <c r="S33" s="9">
+      <c r="S33" s="5">
         <f t="shared" si="7"/>
         <v>142.53800000000001</v>
       </c>
-      <c r="T33" s="9">
+      <c r="T33" s="5">
         <f t="shared" si="8"/>
         <v>113.56</v>
       </c>
-      <c r="U33" s="9">
+      <c r="U33" s="5">
         <f t="shared" si="9"/>
         <v>125.407</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>484508</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>294058</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>219747</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>210850</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>198178</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>217164</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
         <v>232882</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <v>193565</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>157731</v>
       </c>
-      <c r="L34" s="2" t="s">
+      <c r="L34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M34" s="9">
+      <c r="M34" s="5">
         <f t="shared" si="1"/>
         <v>484.50799999999998</v>
       </c>
-      <c r="N34" s="9">
+      <c r="N34" s="5">
         <f t="shared" si="2"/>
         <v>294.05799999999999</v>
       </c>
-      <c r="O34" s="9">
+      <c r="O34" s="5">
         <f t="shared" si="3"/>
         <v>219.74700000000001</v>
       </c>
-      <c r="P34" s="9">
+      <c r="P34" s="5">
         <f t="shared" si="4"/>
         <v>210.85</v>
       </c>
-      <c r="Q34" s="9">
+      <c r="Q34" s="5">
         <f t="shared" si="5"/>
         <v>198.178</v>
       </c>
-      <c r="R34" s="9">
+      <c r="R34" s="5">
         <f t="shared" si="6"/>
         <v>217.16399999999999</v>
       </c>
-      <c r="S34" s="9">
+      <c r="S34" s="5">
         <f t="shared" si="7"/>
         <v>232.88200000000001</v>
       </c>
-      <c r="T34" s="9">
+      <c r="T34" s="5">
         <f t="shared" si="8"/>
         <v>193.565</v>
       </c>
-      <c r="U34" s="9">
+      <c r="U34" s="5">
         <f t="shared" si="9"/>
         <v>157.73099999999999</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="L35" s="11" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="L35" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="12">
+      <c r="M35" s="8">
         <f xml:space="preserve"> SUM(M30:M34)/60</f>
         <v>17.525750000000002</v>
       </c>
-      <c r="N35" s="12">
+      <c r="N35" s="8">
         <f t="shared" ref="N35:U35" si="10" xml:space="preserve"> SUM(N30:N34)/60</f>
         <v>10.644883333333333</v>
       </c>
-      <c r="O35" s="12">
+      <c r="O35" s="8">
         <f t="shared" si="10"/>
         <v>8.6542333333333339</v>
       </c>
-      <c r="P35" s="12">
+      <c r="P35" s="8">
         <f t="shared" si="10"/>
         <v>7.8352500000000003</v>
       </c>
-      <c r="Q35" s="12">
+      <c r="Q35" s="8">
         <f t="shared" si="10"/>
         <v>7.2229166666666664</v>
       </c>
-      <c r="R35" s="12">
+      <c r="R35" s="8">
         <f t="shared" si="10"/>
         <v>8.3247833333333325</v>
       </c>
-      <c r="S35" s="12">
+      <c r="S35" s="8">
         <f t="shared" si="10"/>
         <v>8.7949166666666656</v>
       </c>
-      <c r="T35" s="12">
+      <c r="T35" s="8">
         <f t="shared" si="10"/>
         <v>7.5955000000000004</v>
       </c>
-      <c r="U35" s="12">
+      <c r="U35" s="8">
         <f t="shared" si="10"/>
         <v>7.6705499999999995</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="M37" s="6" t="s">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="M37" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>76958</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>43054</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>31083</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>22430</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>21305</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>26423</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
         <v>23880</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="1">
         <v>22029</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="1">
         <v>21393</v>
       </c>
-      <c r="L38" s="2" t="s">
+      <c r="L38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M38" s="9">
+      <c r="M38" s="5">
         <f>B38/1000</f>
         <v>76.957999999999998</v>
       </c>
-      <c r="N38" s="9">
+      <c r="N38" s="5">
         <f t="shared" ref="N38:U42" si="11">C38/1000</f>
         <v>43.054000000000002</v>
       </c>
-      <c r="O38" s="9">
+      <c r="O38" s="5">
         <f t="shared" si="11"/>
         <v>31.082999999999998</v>
       </c>
-      <c r="P38" s="9">
+      <c r="P38" s="5">
         <f t="shared" si="11"/>
         <v>22.43</v>
       </c>
-      <c r="Q38" s="9">
+      <c r="Q38" s="5">
         <f t="shared" si="11"/>
         <v>21.305</v>
       </c>
-      <c r="R38" s="9">
+      <c r="R38" s="5">
         <f t="shared" si="11"/>
         <v>26.422999999999998</v>
       </c>
-      <c r="S38" s="9">
+      <c r="S38" s="5">
         <f t="shared" si="11"/>
         <v>23.88</v>
       </c>
-      <c r="T38" s="9">
+      <c r="T38" s="5">
         <f t="shared" si="11"/>
         <v>22.029</v>
       </c>
-      <c r="U38" s="9">
+      <c r="U38" s="5">
         <f t="shared" si="11"/>
         <v>21.393000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>95501</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>51333</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>31995</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>24003</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>21659</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>27118</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="1">
         <v>24389</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="1">
         <v>22192</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="1">
         <v>21479</v>
       </c>
-      <c r="L39" s="2" t="s">
+      <c r="L39" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M39" s="9">
+      <c r="M39" s="5">
         <f t="shared" ref="M39:M42" si="12">B39/1000</f>
         <v>95.501000000000005</v>
       </c>
-      <c r="N39" s="9">
+      <c r="N39" s="5">
         <f t="shared" si="11"/>
         <v>51.332999999999998</v>
       </c>
-      <c r="O39" s="9">
+      <c r="O39" s="5">
         <f t="shared" si="11"/>
         <v>31.995000000000001</v>
       </c>
-      <c r="P39" s="9">
+      <c r="P39" s="5">
         <f t="shared" si="11"/>
         <v>24.003</v>
       </c>
-      <c r="Q39" s="9">
+      <c r="Q39" s="5">
         <f t="shared" si="11"/>
         <v>21.658999999999999</v>
       </c>
-      <c r="R39" s="9">
+      <c r="R39" s="5">
         <f t="shared" si="11"/>
         <v>27.117999999999999</v>
       </c>
-      <c r="S39" s="9">
+      <c r="S39" s="5">
         <f t="shared" si="11"/>
         <v>24.388999999999999</v>
       </c>
-      <c r="T39" s="9">
+      <c r="T39" s="5">
         <f t="shared" si="11"/>
         <v>22.192</v>
       </c>
-      <c r="U39" s="9">
+      <c r="U39" s="5">
         <f t="shared" si="11"/>
         <v>21.478999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>92846</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>49914</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>32258</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>26981</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>21353</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>27508</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="1">
         <v>24780</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="1">
         <v>21989</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="1">
         <v>21387</v>
       </c>
-      <c r="L40" s="2" t="s">
+      <c r="L40" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M40" s="9">
+      <c r="M40" s="5">
         <f t="shared" si="12"/>
         <v>92.846000000000004</v>
       </c>
-      <c r="N40" s="9">
+      <c r="N40" s="5">
         <f t="shared" si="11"/>
         <v>49.914000000000001</v>
       </c>
-      <c r="O40" s="9">
+      <c r="O40" s="5">
         <f t="shared" si="11"/>
         <v>32.258000000000003</v>
       </c>
-      <c r="P40" s="9">
+      <c r="P40" s="5">
         <f t="shared" si="11"/>
         <v>26.981000000000002</v>
       </c>
-      <c r="Q40" s="9">
+      <c r="Q40" s="5">
         <f t="shared" si="11"/>
         <v>21.353000000000002</v>
       </c>
-      <c r="R40" s="9">
+      <c r="R40" s="5">
         <f t="shared" si="11"/>
         <v>27.507999999999999</v>
       </c>
-      <c r="S40" s="9">
+      <c r="S40" s="5">
         <f t="shared" si="11"/>
         <v>24.78</v>
       </c>
-      <c r="T40" s="9">
+      <c r="T40" s="5">
         <f t="shared" si="11"/>
         <v>21.989000000000001</v>
       </c>
-      <c r="U40" s="9">
+      <c r="U40" s="5">
         <f t="shared" si="11"/>
         <v>21.387</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>343710</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>172356</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>115892</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>89541</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>70335</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>91382</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>85606</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="1">
         <v>76412</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="1">
         <v>70268</v>
       </c>
-      <c r="L41" s="2" t="s">
+      <c r="L41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M41" s="9">
+      <c r="M41" s="5">
         <f t="shared" si="12"/>
         <v>343.71</v>
       </c>
-      <c r="N41" s="9">
+      <c r="N41" s="5">
         <f t="shared" si="11"/>
         <v>172.35599999999999</v>
       </c>
-      <c r="O41" s="9">
+      <c r="O41" s="5">
         <f t="shared" si="11"/>
         <v>115.892</v>
       </c>
-      <c r="P41" s="9">
+      <c r="P41" s="5">
         <f t="shared" si="11"/>
         <v>89.540999999999997</v>
       </c>
-      <c r="Q41" s="9">
+      <c r="Q41" s="5">
         <f t="shared" si="11"/>
         <v>70.334999999999994</v>
       </c>
-      <c r="R41" s="9">
+      <c r="R41" s="5">
         <f t="shared" si="11"/>
         <v>91.382000000000005</v>
       </c>
-      <c r="S41" s="9">
+      <c r="S41" s="5">
         <f t="shared" si="11"/>
         <v>85.605999999999995</v>
       </c>
-      <c r="T41" s="9">
+      <c r="T41" s="5">
         <f t="shared" si="11"/>
         <v>76.412000000000006</v>
       </c>
-      <c r="U41" s="9">
+      <c r="U41" s="5">
         <f t="shared" si="11"/>
         <v>70.268000000000001</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>553436</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>291360</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>185700</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>143304</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>112508</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>150613</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>138999</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="1">
         <v>125640</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="1">
         <v>112744</v>
       </c>
-      <c r="L42" s="2" t="s">
+      <c r="L42" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M42" s="9">
+      <c r="M42" s="5">
         <f t="shared" si="12"/>
         <v>553.43600000000004</v>
       </c>
-      <c r="N42" s="9">
+      <c r="N42" s="5">
         <f t="shared" si="11"/>
         <v>291.36</v>
       </c>
-      <c r="O42" s="9">
+      <c r="O42" s="5">
         <f t="shared" si="11"/>
         <v>185.7</v>
       </c>
-      <c r="P42" s="9">
+      <c r="P42" s="5">
         <f t="shared" si="11"/>
         <v>143.304</v>
       </c>
-      <c r="Q42" s="9">
+      <c r="Q42" s="5">
         <f t="shared" si="11"/>
         <v>112.508</v>
       </c>
-      <c r="R42" s="9">
+      <c r="R42" s="5">
         <f t="shared" si="11"/>
         <v>150.613</v>
       </c>
-      <c r="S42" s="9">
+      <c r="S42" s="5">
         <f t="shared" si="11"/>
         <v>138.999</v>
       </c>
-      <c r="T42" s="9">
+      <c r="T42" s="5">
         <f t="shared" si="11"/>
         <v>125.64</v>
       </c>
-      <c r="U42" s="9">
+      <c r="U42" s="5">
         <f t="shared" si="11"/>
         <v>112.744</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="10"/>
-      <c r="F43" s="10"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
-      <c r="J43" s="10"/>
-      <c r="L43" s="11" t="s">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="L43" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M43" s="12">
+      <c r="M43" s="8">
         <f xml:space="preserve"> SUM(M38:M42)/60</f>
         <v>19.374183333333335</v>
       </c>
-      <c r="N43" s="12">
+      <c r="N43" s="8">
         <f t="shared" ref="N43" si="13" xml:space="preserve"> SUM(N38:N42)/60</f>
         <v>10.133616666666667</v>
       </c>
-      <c r="O43" s="12">
+      <c r="O43" s="8">
         <f t="shared" ref="O43" si="14" xml:space="preserve"> SUM(O38:O42)/60</f>
         <v>6.6154666666666664</v>
       </c>
-      <c r="P43" s="12">
+      <c r="P43" s="8">
         <f t="shared" ref="P43" si="15" xml:space="preserve"> SUM(P38:P42)/60</f>
         <v>5.1043166666666666</v>
       </c>
-      <c r="Q43" s="12">
+      <c r="Q43" s="8">
         <f t="shared" ref="Q43" si="16" xml:space="preserve"> SUM(Q38:Q42)/60</f>
         <v>4.1193333333333326</v>
       </c>
-      <c r="R43" s="12">
+      <c r="R43" s="8">
         <f t="shared" ref="R43" si="17" xml:space="preserve"> SUM(R38:R42)/60</f>
         <v>5.3840666666666666</v>
       </c>
-      <c r="S43" s="12">
+      <c r="S43" s="8">
         <f t="shared" ref="S43" si="18" xml:space="preserve"> SUM(S38:S42)/60</f>
         <v>4.9608999999999996</v>
       </c>
-      <c r="T43" s="12">
+      <c r="T43" s="8">
         <f t="shared" ref="T43" si="19" xml:space="preserve"> SUM(T38:T42)/60</f>
         <v>4.4710333333333336</v>
       </c>
-      <c r="U43" s="12">
+      <c r="U43" s="8">
         <f t="shared" ref="U43" si="20" xml:space="preserve"> SUM(U38:U42)/60</f>
         <v>4.1211833333333328</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
+      <c r="A46" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="L46" s="8" t="s">
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="L46" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M46" s="8"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="8"/>
-      <c r="S46" s="8"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="8"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="L47" s="1" t="s">
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="L47" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="T47" s="11"/>
+      <c r="U47" s="11"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>1</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="4">
         <v>2</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="4">
         <v>4</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="4">
         <v>6</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="4">
         <v>8</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="4">
         <v>10</v>
       </c>
-      <c r="H48" s="7">
+      <c r="H48" s="4">
         <v>12</v>
       </c>
-      <c r="I48" s="7">
+      <c r="I48" s="4">
         <v>14</v>
       </c>
-      <c r="J48" s="7">
+      <c r="J48" s="4">
         <v>16</v>
       </c>
-      <c r="M48" s="7">
+      <c r="M48" s="4">
         <v>1</v>
       </c>
-      <c r="N48" s="7">
+      <c r="N48" s="4">
         <v>2</v>
       </c>
-      <c r="O48" s="7">
+      <c r="O48" s="4">
         <v>4</v>
       </c>
-      <c r="P48" s="7">
+      <c r="P48" s="4">
         <v>6</v>
       </c>
-      <c r="Q48" s="7">
+      <c r="Q48" s="4">
         <v>8</v>
       </c>
-      <c r="R48" s="7">
+      <c r="R48" s="4">
         <v>10</v>
       </c>
-      <c r="S48" s="7">
+      <c r="S48" s="4">
         <v>12</v>
       </c>
-      <c r="T48" s="7">
+      <c r="T48" s="4">
         <v>14</v>
       </c>
-      <c r="U48" s="7">
+      <c r="U48" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="M49" s="6" t="s">
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="M49" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6"/>
-      <c r="U49" s="6"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
     </row>
     <row r="50" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B50">
@@ -3714,48 +3723,48 @@
       <c r="J50">
         <v>33281</v>
       </c>
-      <c r="L50" s="2" t="s">
+      <c r="L50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M50" s="9">
+      <c r="M50" s="5">
         <f>B50/1000</f>
         <v>71.203000000000003</v>
       </c>
-      <c r="N50" s="9">
+      <c r="N50" s="5">
         <f t="shared" ref="N50:U54" si="21">C50/1000</f>
         <v>40.999000000000002</v>
       </c>
-      <c r="O50" s="9">
+      <c r="O50" s="5">
         <f t="shared" si="21"/>
         <v>21.856999999999999</v>
       </c>
-      <c r="P50" s="9">
+      <c r="P50" s="5">
         <f t="shared" si="21"/>
         <v>31.388000000000002</v>
       </c>
-      <c r="Q50" s="9">
+      <c r="Q50" s="5">
         <f t="shared" si="21"/>
         <v>25.140999999999998</v>
       </c>
-      <c r="R50" s="9">
+      <c r="R50" s="5">
         <f t="shared" si="21"/>
         <v>34.639000000000003</v>
       </c>
-      <c r="S50" s="9">
+      <c r="S50" s="5">
         <f t="shared" si="21"/>
         <v>32.982999999999997</v>
       </c>
-      <c r="T50" s="9">
+      <c r="T50" s="5">
         <f t="shared" si="21"/>
         <v>33.701000000000001</v>
       </c>
-      <c r="U50" s="9">
+      <c r="U50" s="5">
         <f t="shared" si="21"/>
         <v>33.280999999999999</v>
       </c>
     </row>
     <row r="51" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B51">
@@ -3785,48 +3794,48 @@
       <c r="J51">
         <v>50683</v>
       </c>
-      <c r="L51" s="2" t="s">
+      <c r="L51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M51" s="9">
+      <c r="M51" s="5">
         <f t="shared" ref="M51:M54" si="22">B51/1000</f>
         <v>87.442999999999998</v>
       </c>
-      <c r="N51" s="9">
+      <c r="N51" s="5">
         <f t="shared" si="21"/>
         <v>48.165999999999997</v>
       </c>
-      <c r="O51" s="9">
+      <c r="O51" s="5">
         <f t="shared" si="21"/>
         <v>53.167999999999999</v>
       </c>
-      <c r="P51" s="9">
+      <c r="P51" s="5">
         <f t="shared" si="21"/>
         <v>43.558999999999997</v>
       </c>
-      <c r="Q51" s="9">
+      <c r="Q51" s="5">
         <f t="shared" si="21"/>
         <v>42.046999999999997</v>
       </c>
-      <c r="R51" s="9">
+      <c r="R51" s="5">
         <f t="shared" si="21"/>
         <v>53.122999999999998</v>
       </c>
-      <c r="S51" s="9">
+      <c r="S51" s="5">
         <f t="shared" si="21"/>
         <v>54.48</v>
       </c>
-      <c r="T51" s="9">
+      <c r="T51" s="5">
         <f t="shared" si="21"/>
         <v>51.872</v>
       </c>
-      <c r="U51" s="9">
+      <c r="U51" s="5">
         <f t="shared" si="21"/>
         <v>50.683</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B52">
@@ -3856,48 +3865,48 @@
       <c r="J52">
         <v>92860</v>
       </c>
-      <c r="L52" s="2" t="s">
+      <c r="L52" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M52" s="9">
+      <c r="M52" s="5">
         <f t="shared" si="22"/>
         <v>89.168999999999997</v>
       </c>
-      <c r="N52" s="9">
+      <c r="N52" s="5">
         <f t="shared" si="21"/>
         <v>52.917000000000002</v>
       </c>
-      <c r="O52" s="9">
+      <c r="O52" s="5">
         <f t="shared" si="21"/>
         <v>63.576999999999998</v>
       </c>
-      <c r="P52" s="9">
+      <c r="P52" s="5">
         <f t="shared" si="21"/>
         <v>67.123000000000005</v>
       </c>
-      <c r="Q52" s="9">
+      <c r="Q52" s="5">
         <f t="shared" si="21"/>
         <v>73.641999999999996</v>
       </c>
-      <c r="R52" s="9">
+      <c r="R52" s="5">
         <f t="shared" si="21"/>
         <v>87.161000000000001</v>
       </c>
-      <c r="S52" s="9">
+      <c r="S52" s="5">
         <f t="shared" si="21"/>
         <v>92.724999999999994</v>
       </c>
-      <c r="T52" s="9">
+      <c r="T52" s="5">
         <f t="shared" si="21"/>
         <v>89.594999999999999</v>
       </c>
-      <c r="U52" s="9">
+      <c r="U52" s="5">
         <f t="shared" si="21"/>
         <v>92.86</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B53">
@@ -3927,48 +3936,48 @@
       <c r="J53">
         <v>158495</v>
       </c>
-      <c r="L53" s="2" t="s">
+      <c r="L53" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M53" s="9">
+      <c r="M53" s="5">
         <f t="shared" si="22"/>
         <v>272.85899999999998</v>
       </c>
-      <c r="N53" s="9">
+      <c r="N53" s="5">
         <f t="shared" si="21"/>
         <v>177.96600000000001</v>
       </c>
-      <c r="O53" s="9">
+      <c r="O53" s="5">
         <f t="shared" si="21"/>
         <v>113.877</v>
       </c>
-      <c r="P53" s="9">
+      <c r="P53" s="5">
         <f t="shared" si="21"/>
         <v>135.892</v>
       </c>
-      <c r="Q53" s="9">
+      <c r="Q53" s="5">
         <f t="shared" si="21"/>
         <v>131.49299999999999</v>
       </c>
-      <c r="R53" s="9">
+      <c r="R53" s="5">
         <f t="shared" si="21"/>
         <v>168.65899999999999</v>
       </c>
-      <c r="S53" s="9">
+      <c r="S53" s="5">
         <f t="shared" si="21"/>
         <v>169.55199999999999</v>
       </c>
-      <c r="T53" s="9">
+      <c r="T53" s="5">
         <f t="shared" si="21"/>
         <v>171.41200000000001</v>
       </c>
-      <c r="U53" s="9">
+      <c r="U53" s="5">
         <f t="shared" si="21"/>
         <v>158.495</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B54">
@@ -3998,114 +4007,114 @@
       <c r="J54">
         <v>256342</v>
       </c>
-      <c r="L54" s="2" t="s">
+      <c r="L54" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M54" s="9">
+      <c r="M54" s="5">
         <f t="shared" si="22"/>
         <v>449.57299999999998</v>
       </c>
-      <c r="N54" s="9">
+      <c r="N54" s="5">
         <f t="shared" si="21"/>
         <v>244.624</v>
       </c>
-      <c r="O54" s="9">
+      <c r="O54" s="5">
         <f t="shared" si="21"/>
         <v>210.81200000000001</v>
       </c>
-      <c r="P54" s="9">
+      <c r="P54" s="5">
         <f t="shared" si="21"/>
         <v>194.09800000000001</v>
       </c>
-      <c r="Q54" s="9">
+      <c r="Q54" s="5">
         <f t="shared" si="21"/>
         <v>251.88300000000001</v>
       </c>
-      <c r="R54" s="9">
+      <c r="R54" s="5">
         <f t="shared" si="21"/>
         <v>255.262</v>
       </c>
-      <c r="S54" s="9">
+      <c r="S54" s="5">
         <f t="shared" si="21"/>
         <v>262.62</v>
       </c>
-      <c r="T54" s="9">
+      <c r="T54" s="5">
         <f t="shared" si="21"/>
         <v>259.899</v>
       </c>
-      <c r="U54" s="9">
+      <c r="U54" s="5">
         <f t="shared" si="21"/>
         <v>256.34199999999998</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="10"/>
-      <c r="L55" s="11" t="s">
+      <c r="A55" s="6"/>
+      <c r="L55" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M55" s="12">
+      <c r="M55" s="8">
         <f xml:space="preserve"> SUM(M50:M54)/60</f>
         <v>16.170783333333333</v>
       </c>
-      <c r="N55" s="12">
+      <c r="N55" s="8">
         <f t="shared" ref="N55" si="23" xml:space="preserve"> SUM(N50:N54)/60</f>
         <v>9.4112000000000009</v>
       </c>
-      <c r="O55" s="12">
+      <c r="O55" s="8">
         <f t="shared" ref="O55" si="24" xml:space="preserve"> SUM(O50:O54)/60</f>
         <v>7.721516666666667</v>
       </c>
-      <c r="P55" s="12">
+      <c r="P55" s="8">
         <f t="shared" ref="P55" si="25" xml:space="preserve"> SUM(P50:P54)/60</f>
         <v>7.8676666666666666</v>
       </c>
-      <c r="Q55" s="12">
+      <c r="Q55" s="8">
         <f t="shared" ref="Q55" si="26" xml:space="preserve"> SUM(Q50:Q54)/60</f>
         <v>8.7367666666666661</v>
       </c>
-      <c r="R55" s="12">
+      <c r="R55" s="8">
         <f t="shared" ref="R55" si="27" xml:space="preserve"> SUM(R50:R54)/60</f>
         <v>9.980733333333335</v>
       </c>
-      <c r="S55" s="12">
+      <c r="S55" s="8">
         <f t="shared" ref="S55" si="28" xml:space="preserve"> SUM(S50:S54)/60</f>
         <v>10.206</v>
       </c>
-      <c r="T55" s="12">
+      <c r="T55" s="8">
         <f t="shared" ref="T55" si="29" xml:space="preserve"> SUM(T50:T54)/60</f>
         <v>10.107983333333333</v>
       </c>
-      <c r="U55" s="12">
+      <c r="U55" s="8">
         <f t="shared" ref="U55" si="30" xml:space="preserve"> SUM(U50:U54)/60</f>
         <v>9.8610166666666679</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
-      <c r="M57" s="6" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="M57" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N57" s="6"/>
-      <c r="O57" s="6"/>
-      <c r="P57" s="6"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
-      <c r="S57" s="6"/>
-      <c r="T57" s="6"/>
-      <c r="U57" s="6"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
+      <c r="R57" s="9"/>
+      <c r="S57" s="9"/>
+      <c r="T57" s="9"/>
+      <c r="U57" s="9"/>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B58">
@@ -4135,48 +4144,48 @@
       <c r="J58">
         <v>27228</v>
       </c>
-      <c r="L58" s="2" t="s">
+      <c r="L58" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M58" s="9">
+      <c r="M58" s="5">
         <f>B58/1000</f>
         <v>76.483000000000004</v>
       </c>
-      <c r="N58" s="9">
+      <c r="N58" s="5">
         <f t="shared" ref="N58:U62" si="31">C58/1000</f>
         <v>41.478999999999999</v>
       </c>
-      <c r="O58" s="9">
+      <c r="O58" s="5">
         <f t="shared" si="31"/>
         <v>21.841999999999999</v>
       </c>
-      <c r="P58" s="9">
+      <c r="P58" s="5">
         <f t="shared" si="31"/>
         <v>29.015999999999998</v>
       </c>
-      <c r="Q58" s="9">
+      <c r="Q58" s="5">
         <f t="shared" si="31"/>
         <v>30.402000000000001</v>
       </c>
-      <c r="R58" s="9">
+      <c r="R58" s="5">
         <f t="shared" si="31"/>
         <v>30.69</v>
       </c>
-      <c r="S58" s="9">
+      <c r="S58" s="5">
         <f t="shared" si="31"/>
         <v>27.434999999999999</v>
       </c>
-      <c r="T58" s="9">
+      <c r="T58" s="5">
         <f t="shared" si="31"/>
         <v>29.408000000000001</v>
       </c>
-      <c r="U58" s="9">
+      <c r="U58" s="5">
         <f t="shared" si="31"/>
         <v>27.228000000000002</v>
       </c>
     </row>
     <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B59">
@@ -4206,48 +4215,48 @@
       <c r="J59">
         <v>29336</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="L59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M59" s="9">
+      <c r="M59" s="5">
         <f t="shared" ref="M59:M62" si="32">B59/1000</f>
         <v>90.929000000000002</v>
       </c>
-      <c r="N59" s="9">
+      <c r="N59" s="5">
         <f t="shared" si="31"/>
         <v>45.570999999999998</v>
       </c>
-      <c r="O59" s="9">
+      <c r="O59" s="5">
         <f t="shared" si="31"/>
         <v>25.637</v>
       </c>
-      <c r="P59" s="9">
+      <c r="P59" s="5">
         <f t="shared" si="31"/>
         <v>30.567</v>
       </c>
-      <c r="Q59" s="9">
+      <c r="Q59" s="5">
         <f t="shared" si="31"/>
         <v>30.576000000000001</v>
       </c>
-      <c r="R59" s="9">
+      <c r="R59" s="5">
         <f t="shared" si="31"/>
         <v>33.238999999999997</v>
       </c>
-      <c r="S59" s="9">
+      <c r="S59" s="5">
         <f t="shared" si="31"/>
         <v>28.681000000000001</v>
       </c>
-      <c r="T59" s="9">
+      <c r="T59" s="5">
         <f t="shared" si="31"/>
         <v>31.084</v>
       </c>
-      <c r="U59" s="9">
+      <c r="U59" s="5">
         <f t="shared" si="31"/>
         <v>29.335999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B60">
@@ -4277,48 +4286,48 @@
       <c r="J60">
         <v>30875</v>
       </c>
-      <c r="L60" s="2" t="s">
+      <c r="L60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M60" s="9">
+      <c r="M60" s="5">
         <f t="shared" si="32"/>
         <v>91.442999999999998</v>
       </c>
-      <c r="N60" s="9">
+      <c r="N60" s="5">
         <f t="shared" si="31"/>
         <v>49.186999999999998</v>
       </c>
-      <c r="O60" s="9">
+      <c r="O60" s="5">
         <f t="shared" si="31"/>
         <v>30.768000000000001</v>
       </c>
-      <c r="P60" s="9">
+      <c r="P60" s="5">
         <f t="shared" si="31"/>
         <v>34.468000000000004</v>
       </c>
-      <c r="Q60" s="9">
+      <c r="Q60" s="5">
         <f t="shared" si="31"/>
         <v>33.225999999999999</v>
       </c>
-      <c r="R60" s="9">
+      <c r="R60" s="5">
         <f t="shared" si="31"/>
         <v>35.659999999999997</v>
       </c>
-      <c r="S60" s="9">
+      <c r="S60" s="5">
         <f t="shared" si="31"/>
         <v>31.056000000000001</v>
       </c>
-      <c r="T60" s="9">
+      <c r="T60" s="5">
         <f t="shared" si="31"/>
         <v>33.947000000000003</v>
       </c>
-      <c r="U60" s="9">
+      <c r="U60" s="5">
         <f t="shared" si="31"/>
         <v>30.875</v>
       </c>
     </row>
     <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B61">
@@ -4348,48 +4357,48 @@
       <c r="J61">
         <v>114171</v>
       </c>
-      <c r="L61" s="2" t="s">
+      <c r="L61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M61" s="9">
+      <c r="M61" s="5">
         <f t="shared" si="32"/>
         <v>336.58699999999999</v>
       </c>
-      <c r="N61" s="9">
+      <c r="N61" s="5">
         <f t="shared" si="31"/>
         <v>173.15299999999999</v>
       </c>
-      <c r="O61" s="9">
+      <c r="O61" s="5">
         <f t="shared" si="31"/>
         <v>115.155</v>
       </c>
-      <c r="P61" s="9">
+      <c r="P61" s="5">
         <f t="shared" si="31"/>
         <v>131.148</v>
       </c>
-      <c r="Q61" s="9">
+      <c r="Q61" s="5">
         <f t="shared" si="31"/>
         <v>116.399</v>
       </c>
-      <c r="R61" s="9">
+      <c r="R61" s="5">
         <f t="shared" si="31"/>
         <v>129.80799999999999</v>
       </c>
-      <c r="S61" s="9">
+      <c r="S61" s="5">
         <f t="shared" si="31"/>
         <v>114.539</v>
       </c>
-      <c r="T61" s="9">
+      <c r="T61" s="5">
         <f t="shared" si="31"/>
         <v>123.31399999999999</v>
       </c>
-      <c r="U61" s="9">
+      <c r="U61" s="5">
         <f t="shared" si="31"/>
         <v>114.17100000000001</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B62">
@@ -4419,221 +4428,221 @@
       <c r="J62">
         <v>186308</v>
       </c>
-      <c r="L62" s="2" t="s">
+      <c r="L62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M62" s="9">
+      <c r="M62" s="5">
         <f t="shared" si="32"/>
         <v>548.00400000000002</v>
       </c>
-      <c r="N62" s="9">
+      <c r="N62" s="5">
         <f t="shared" si="31"/>
         <v>287.45999999999998</v>
       </c>
-      <c r="O62" s="9">
+      <c r="O62" s="5">
         <f t="shared" si="31"/>
         <v>185.917</v>
       </c>
-      <c r="P62" s="9">
+      <c r="P62" s="5">
         <f t="shared" si="31"/>
         <v>221.06399999999999</v>
       </c>
-      <c r="Q62" s="9">
+      <c r="Q62" s="5">
         <f t="shared" si="31"/>
         <v>185.77500000000001</v>
       </c>
-      <c r="R62" s="9">
+      <c r="R62" s="5">
         <f t="shared" si="31"/>
         <v>206.38800000000001</v>
       </c>
-      <c r="S62" s="9">
+      <c r="S62" s="5">
         <f t="shared" si="31"/>
         <v>188.17699999999999</v>
       </c>
-      <c r="T62" s="9">
+      <c r="T62" s="5">
         <f t="shared" si="31"/>
         <v>199.892</v>
       </c>
-      <c r="U62" s="9">
+      <c r="U62" s="5">
         <f t="shared" si="31"/>
         <v>186.30799999999999</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L63" s="11" t="s">
+      <c r="L63" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M63" s="12">
+      <c r="M63" s="8">
         <f xml:space="preserve"> SUM(M58:M62)/60</f>
         <v>19.057433333333332</v>
       </c>
-      <c r="N63" s="12">
+      <c r="N63" s="8">
         <f t="shared" ref="N63" si="33" xml:space="preserve"> SUM(N58:N62)/60</f>
         <v>9.947499999999998</v>
       </c>
-      <c r="O63" s="12">
+      <c r="O63" s="8">
         <f t="shared" ref="O63" si="34" xml:space="preserve"> SUM(O58:O62)/60</f>
         <v>6.3219833333333328</v>
       </c>
-      <c r="P63" s="12">
+      <c r="P63" s="8">
         <f t="shared" ref="P63" si="35" xml:space="preserve"> SUM(P58:P62)/60</f>
         <v>7.4377166666666676</v>
       </c>
-      <c r="Q63" s="12">
+      <c r="Q63" s="8">
         <f t="shared" ref="Q63" si="36" xml:space="preserve"> SUM(Q58:Q62)/60</f>
         <v>6.6063000000000009</v>
       </c>
-      <c r="R63" s="12">
+      <c r="R63" s="8">
         <f t="shared" ref="R63" si="37" xml:space="preserve"> SUM(R58:R62)/60</f>
         <v>7.2630833333333324</v>
       </c>
-      <c r="S63" s="12">
+      <c r="S63" s="8">
         <f t="shared" ref="S63" si="38" xml:space="preserve"> SUM(S58:S62)/60</f>
         <v>6.4981333333333335</v>
       </c>
-      <c r="T63" s="12">
+      <c r="T63" s="8">
         <f t="shared" ref="T63" si="39" xml:space="preserve"> SUM(T58:T62)/60</f>
         <v>6.96075</v>
       </c>
-      <c r="U63" s="12">
+      <c r="U63" s="8">
         <f t="shared" ref="U63" si="40" xml:space="preserve"> SUM(U58:U62)/60</f>
         <v>6.4653</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A65" s="8" t="s">
+      <c r="A65" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="L65" s="8" t="s">
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="L65" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="M65" s="8"/>
-      <c r="N65" s="8"/>
-      <c r="O65" s="8"/>
-      <c r="P65" s="8"/>
-      <c r="Q65" s="8"/>
-      <c r="R65" s="8"/>
-      <c r="S65" s="8"/>
-      <c r="T65" s="8"/>
-      <c r="U65" s="8"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
+      <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="L66" s="1" t="s">
+      <c r="B66" s="11"/>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="L66" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-      <c r="O66" s="1"/>
-      <c r="P66" s="1"/>
-      <c r="Q66" s="1"/>
-      <c r="R66" s="1"/>
-      <c r="S66" s="1"/>
-      <c r="T66" s="1"/>
-      <c r="U66" s="1"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="11"/>
+      <c r="O66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="Q66" s="11"/>
+      <c r="R66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="T66" s="11"/>
+      <c r="U66" s="11"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B67" s="7">
+      <c r="B67" s="4">
         <v>1</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="4">
         <v>2</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D67" s="4">
         <v>4</v>
       </c>
-      <c r="E67" s="7">
+      <c r="E67" s="4">
         <v>6</v>
       </c>
-      <c r="F67" s="7">
+      <c r="F67" s="4">
         <v>8</v>
       </c>
-      <c r="G67" s="7">
+      <c r="G67" s="4">
         <v>10</v>
       </c>
-      <c r="H67" s="7">
+      <c r="H67" s="4">
         <v>12</v>
       </c>
-      <c r="I67" s="7">
+      <c r="I67" s="4">
         <v>14</v>
       </c>
-      <c r="J67" s="7">
+      <c r="J67" s="4">
         <v>16</v>
       </c>
-      <c r="M67" s="7">
+      <c r="M67" s="4">
         <v>1</v>
       </c>
-      <c r="N67" s="7">
+      <c r="N67" s="4">
         <v>2</v>
       </c>
-      <c r="O67" s="7">
+      <c r="O67" s="4">
         <v>4</v>
       </c>
-      <c r="P67" s="7">
+      <c r="P67" s="4">
         <v>6</v>
       </c>
-      <c r="Q67" s="7">
+      <c r="Q67" s="4">
         <v>8</v>
       </c>
-      <c r="R67" s="7">
+      <c r="R67" s="4">
         <v>10</v>
       </c>
-      <c r="S67" s="7">
+      <c r="S67" s="4">
         <v>12</v>
       </c>
-      <c r="T67" s="7">
+      <c r="T67" s="4">
         <v>14</v>
       </c>
-      <c r="U67" s="7">
+      <c r="U67" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="F68" s="6"/>
-      <c r="G68" s="6"/>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="M68" s="6" t="s">
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="M68" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="N68" s="6"/>
-      <c r="O68" s="6"/>
-      <c r="P68" s="6"/>
-      <c r="Q68" s="6"/>
-      <c r="R68" s="6"/>
-      <c r="S68" s="6"/>
-      <c r="T68" s="6"/>
-      <c r="U68" s="6"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="9"/>
+      <c r="U68" s="9"/>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B69">
@@ -4663,48 +4672,48 @@
       <c r="J69">
         <v>24472</v>
       </c>
-      <c r="L69" s="2" t="s">
+      <c r="L69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M69" s="9">
+      <c r="M69" s="5">
         <f>B69/1000</f>
         <v>73.093999999999994</v>
       </c>
-      <c r="N69" s="9">
+      <c r="N69" s="5">
         <f t="shared" ref="N69:U73" si="41">C69/1000</f>
         <v>39.811999999999998</v>
       </c>
-      <c r="O69" s="9">
+      <c r="O69" s="5">
         <f t="shared" si="41"/>
         <v>26.29</v>
       </c>
-      <c r="P69" s="9">
+      <c r="P69" s="5">
         <f t="shared" si="41"/>
         <v>25.503</v>
       </c>
-      <c r="Q69" s="9">
+      <c r="Q69" s="5">
         <f t="shared" si="41"/>
         <v>21.966999999999999</v>
       </c>
-      <c r="R69" s="9">
+      <c r="R69" s="5">
         <f t="shared" si="41"/>
         <v>22.207999999999998</v>
       </c>
-      <c r="S69" s="9">
+      <c r="S69" s="5">
         <f t="shared" si="41"/>
         <v>25.138000000000002</v>
       </c>
-      <c r="T69" s="9">
+      <c r="T69" s="5">
         <f t="shared" si="41"/>
         <v>34.32</v>
       </c>
-      <c r="U69" s="9">
+      <c r="U69" s="5">
         <f t="shared" si="41"/>
         <v>24.472000000000001</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B70">
@@ -4734,48 +4743,48 @@
       <c r="J70">
         <v>51421</v>
       </c>
-      <c r="L70" s="2" t="s">
+      <c r="L70" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M70" s="9">
+      <c r="M70" s="5">
         <f t="shared" ref="M70:M73" si="42">B70/1000</f>
         <v>183.404</v>
       </c>
-      <c r="N70" s="9">
+      <c r="N70" s="5">
         <f t="shared" si="41"/>
         <v>98.587999999999994</v>
       </c>
-      <c r="O70" s="9">
+      <c r="O70" s="5">
         <f t="shared" si="41"/>
         <v>64.831999999999994</v>
       </c>
-      <c r="P70" s="9">
+      <c r="P70" s="5">
         <f t="shared" si="41"/>
         <v>47.890999999999998</v>
       </c>
-      <c r="Q70" s="9">
+      <c r="Q70" s="5">
         <f t="shared" si="41"/>
         <v>46.750999999999998</v>
       </c>
-      <c r="R70" s="9">
+      <c r="R70" s="5">
         <f t="shared" si="41"/>
         <v>57.152999999999999</v>
       </c>
-      <c r="S70" s="9">
+      <c r="S70" s="5">
         <f t="shared" si="41"/>
         <v>52.610999999999997</v>
       </c>
-      <c r="T70" s="9">
+      <c r="T70" s="5">
         <f t="shared" si="41"/>
         <v>48.564999999999998</v>
       </c>
-      <c r="U70" s="9">
+      <c r="U70" s="5">
         <f t="shared" si="41"/>
         <v>51.420999999999999</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B71">
@@ -4805,48 +4814,48 @@
       <c r="J71">
         <v>58992</v>
       </c>
-      <c r="L71" s="2" t="s">
+      <c r="L71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M71" s="9">
+      <c r="M71" s="5">
         <f t="shared" si="42"/>
         <v>224.19300000000001</v>
       </c>
-      <c r="N71" s="9">
+      <c r="N71" s="5">
         <f t="shared" si="41"/>
         <v>118.60299999999999</v>
       </c>
-      <c r="O71" s="9">
+      <c r="O71" s="5">
         <f t="shared" si="41"/>
         <v>78.317999999999998</v>
       </c>
-      <c r="P71" s="9">
+      <c r="P71" s="5">
         <f t="shared" si="41"/>
         <v>67.468000000000004</v>
       </c>
-      <c r="Q71" s="9">
+      <c r="Q71" s="5">
         <f t="shared" si="41"/>
         <v>66.501999999999995</v>
       </c>
-      <c r="R71" s="9">
+      <c r="R71" s="5">
         <f t="shared" si="41"/>
         <v>72.435000000000002</v>
       </c>
-      <c r="S71" s="9">
+      <c r="S71" s="5">
         <f t="shared" si="41"/>
         <v>81.93</v>
       </c>
-      <c r="T71" s="9">
+      <c r="T71" s="5">
         <f t="shared" si="41"/>
         <v>72.427999999999997</v>
       </c>
-      <c r="U71" s="9">
+      <c r="U71" s="5">
         <f t="shared" si="41"/>
         <v>58.991999999999997</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B72">
@@ -4876,48 +4885,48 @@
       <c r="J72">
         <v>136137</v>
       </c>
-      <c r="L72" s="2" t="s">
+      <c r="L72" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M72" s="9">
+      <c r="M72" s="5">
         <f t="shared" si="42"/>
         <v>515.21299999999997</v>
       </c>
-      <c r="N72" s="9">
+      <c r="N72" s="5">
         <f t="shared" si="41"/>
         <v>208.05799999999999</v>
       </c>
-      <c r="O72" s="9">
+      <c r="O72" s="5">
         <f t="shared" si="41"/>
         <v>155.11699999999999</v>
       </c>
-      <c r="P72" s="9">
+      <c r="P72" s="5">
         <f t="shared" si="41"/>
         <v>141.38499999999999</v>
       </c>
-      <c r="Q72" s="9">
+      <c r="Q72" s="5">
         <f t="shared" si="41"/>
         <v>113.33199999999999</v>
       </c>
-      <c r="R72" s="9">
+      <c r="R72" s="5">
         <f t="shared" si="41"/>
         <v>117.566</v>
       </c>
-      <c r="S72" s="9">
+      <c r="S72" s="5">
         <f t="shared" si="41"/>
         <v>121.974</v>
       </c>
-      <c r="T72" s="9">
+      <c r="T72" s="5">
         <f t="shared" si="41"/>
         <v>149.1</v>
       </c>
-      <c r="U72" s="9">
+      <c r="U72" s="5">
         <f t="shared" si="41"/>
         <v>136.137</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B73">
@@ -4947,114 +4956,114 @@
       <c r="J73">
         <v>172319</v>
       </c>
-      <c r="L73" s="2" t="s">
+      <c r="L73" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M73" s="9">
+      <c r="M73" s="5">
         <f t="shared" si="42"/>
         <v>851.50400000000002</v>
       </c>
-      <c r="N73" s="9">
+      <c r="N73" s="5">
         <f t="shared" si="41"/>
         <v>361.09800000000001</v>
       </c>
-      <c r="O73" s="9">
+      <c r="O73" s="5">
         <f t="shared" si="41"/>
         <v>315.12</v>
       </c>
-      <c r="P73" s="9">
+      <c r="P73" s="5">
         <f t="shared" si="41"/>
         <v>227.50700000000001</v>
       </c>
-      <c r="Q73" s="9">
+      <c r="Q73" s="5">
         <f t="shared" si="41"/>
         <v>247.65600000000001</v>
       </c>
-      <c r="R73" s="9">
+      <c r="R73" s="5">
         <f t="shared" si="41"/>
         <v>238.44300000000001</v>
       </c>
-      <c r="S73" s="9">
+      <c r="S73" s="5">
         <f t="shared" si="41"/>
         <v>267.24</v>
       </c>
-      <c r="T73" s="9">
+      <c r="T73" s="5">
         <f t="shared" si="41"/>
         <v>270.62700000000001</v>
       </c>
-      <c r="U73" s="9">
+      <c r="U73" s="5">
         <f t="shared" si="41"/>
         <v>172.31899999999999</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="L74" s="11" t="s">
+      <c r="A74" s="6"/>
+      <c r="L74" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M74" s="12">
+      <c r="M74" s="8">
         <f xml:space="preserve"> SUM(M69:M73)/60</f>
         <v>30.790133333333333</v>
       </c>
-      <c r="N74" s="12">
+      <c r="N74" s="8">
         <f t="shared" ref="N74" si="43" xml:space="preserve"> SUM(N69:N73)/60</f>
         <v>13.769316666666667</v>
       </c>
-      <c r="O74" s="12">
+      <c r="O74" s="8">
         <f t="shared" ref="O74" si="44" xml:space="preserve"> SUM(O69:O73)/60</f>
         <v>10.661283333333333</v>
       </c>
-      <c r="P74" s="12">
+      <c r="P74" s="8">
         <f t="shared" ref="P74" si="45" xml:space="preserve"> SUM(P69:P73)/60</f>
         <v>8.4959000000000007</v>
       </c>
-      <c r="Q74" s="12">
+      <c r="Q74" s="8">
         <f t="shared" ref="Q74" si="46" xml:space="preserve"> SUM(Q69:Q73)/60</f>
         <v>8.270133333333332</v>
       </c>
-      <c r="R74" s="12">
+      <c r="R74" s="8">
         <f t="shared" ref="R74" si="47" xml:space="preserve"> SUM(R69:R73)/60</f>
         <v>8.4634166666666655</v>
       </c>
-      <c r="S74" s="12">
+      <c r="S74" s="8">
         <f t="shared" ref="S74" si="48" xml:space="preserve"> SUM(S69:S73)/60</f>
         <v>9.1482166666666664</v>
       </c>
-      <c r="T74" s="12">
+      <c r="T74" s="8">
         <f t="shared" ref="T74" si="49" xml:space="preserve"> SUM(T69:T73)/60</f>
         <v>9.5839999999999996</v>
       </c>
-      <c r="U74" s="12">
+      <c r="U74" s="8">
         <f t="shared" ref="U74" si="50" xml:space="preserve"> SUM(U69:U73)/60</f>
         <v>7.3890166666666666</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C76" s="6"/>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
-      <c r="F76" s="6"/>
-      <c r="G76" s="6"/>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="M76" s="6" t="s">
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="M76" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N76" s="6"/>
-      <c r="O76" s="6"/>
-      <c r="P76" s="6"/>
-      <c r="Q76" s="6"/>
-      <c r="R76" s="6"/>
-      <c r="S76" s="6"/>
-      <c r="T76" s="6"/>
-      <c r="U76" s="6"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="9"/>
+      <c r="S76" s="9"/>
+      <c r="T76" s="9"/>
+      <c r="U76" s="9"/>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B77">
@@ -5084,48 +5093,48 @@
       <c r="J77">
         <v>21377</v>
       </c>
-      <c r="L77" s="2" t="s">
+      <c r="L77" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M77" s="9">
+      <c r="M77" s="5">
         <f>B77/1000</f>
         <v>79.11</v>
       </c>
-      <c r="N77" s="9">
+      <c r="N77" s="5">
         <f t="shared" ref="N77:U81" si="51">C77/1000</f>
         <v>42.515999999999998</v>
       </c>
-      <c r="O77" s="9">
+      <c r="O77" s="5">
         <f t="shared" si="51"/>
         <v>26.65</v>
       </c>
-      <c r="P77" s="9">
+      <c r="P77" s="5">
         <f t="shared" si="51"/>
         <v>23.524000000000001</v>
       </c>
-      <c r="Q77" s="9">
+      <c r="Q77" s="5">
         <f t="shared" si="51"/>
         <v>21.311</v>
       </c>
-      <c r="R77" s="9">
+      <c r="R77" s="5">
         <f t="shared" si="51"/>
         <v>21.404</v>
       </c>
-      <c r="S77" s="9">
+      <c r="S77" s="5">
         <f t="shared" si="51"/>
         <v>21.37</v>
       </c>
-      <c r="T77" s="9">
+      <c r="T77" s="5">
         <f t="shared" si="51"/>
         <v>21.544</v>
       </c>
-      <c r="U77" s="9">
+      <c r="U77" s="5">
         <f t="shared" si="51"/>
         <v>21.376999999999999</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B78">
@@ -5155,48 +5164,48 @@
       <c r="J78">
         <v>21879</v>
       </c>
-      <c r="L78" s="2" t="s">
+      <c r="L78" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M78" s="9">
+      <c r="M78" s="5">
         <f t="shared" ref="M78:M81" si="52">B78/1000</f>
         <v>83.906999999999996</v>
       </c>
-      <c r="N78" s="9">
+      <c r="N78" s="5">
         <f t="shared" si="51"/>
         <v>44.137999999999998</v>
       </c>
-      <c r="O78" s="9">
+      <c r="O78" s="5">
         <f t="shared" si="51"/>
         <v>47.878999999999998</v>
       </c>
-      <c r="P78" s="9">
+      <c r="P78" s="5">
         <f t="shared" si="51"/>
         <v>25.088000000000001</v>
       </c>
-      <c r="Q78" s="9">
+      <c r="Q78" s="5">
         <f t="shared" si="51"/>
         <v>21.62</v>
       </c>
-      <c r="R78" s="9">
+      <c r="R78" s="5">
         <f t="shared" si="51"/>
         <v>26.4</v>
       </c>
-      <c r="S78" s="9">
+      <c r="S78" s="5">
         <f t="shared" si="51"/>
         <v>21.852</v>
       </c>
-      <c r="T78" s="9">
+      <c r="T78" s="5">
         <f t="shared" si="51"/>
         <v>21.634</v>
       </c>
-      <c r="U78" s="9">
+      <c r="U78" s="5">
         <f t="shared" si="51"/>
         <v>21.879000000000001</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B79">
@@ -5226,48 +5235,48 @@
       <c r="J79">
         <v>21373</v>
       </c>
-      <c r="L79" s="2" t="s">
+      <c r="L79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M79" s="9">
+      <c r="M79" s="5">
         <f t="shared" si="52"/>
         <v>91.15</v>
       </c>
-      <c r="N79" s="9">
+      <c r="N79" s="5">
         <f t="shared" si="51"/>
         <v>44.795999999999999</v>
       </c>
-      <c r="O79" s="9">
+      <c r="O79" s="5">
         <f t="shared" si="51"/>
         <v>32.283999999999999</v>
       </c>
-      <c r="P79" s="9">
+      <c r="P79" s="5">
         <f t="shared" si="51"/>
         <v>26.196000000000002</v>
       </c>
-      <c r="Q79" s="9">
+      <c r="Q79" s="5">
         <f t="shared" si="51"/>
         <v>21.393000000000001</v>
       </c>
-      <c r="R79" s="9">
+      <c r="R79" s="5">
         <f t="shared" si="51"/>
         <v>21.617999999999999</v>
       </c>
-      <c r="S79" s="9">
+      <c r="S79" s="5">
         <f t="shared" si="51"/>
         <v>23.521000000000001</v>
       </c>
-      <c r="T79" s="9">
+      <c r="T79" s="5">
         <f t="shared" si="51"/>
         <v>21.622</v>
       </c>
-      <c r="U79" s="9">
+      <c r="U79" s="5">
         <f t="shared" si="51"/>
         <v>21.373000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B80">
@@ -5297,48 +5306,48 @@
       <c r="J80">
         <v>71619</v>
       </c>
-      <c r="L80" s="2" t="s">
+      <c r="L80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M80" s="9">
+      <c r="M80" s="5">
         <f t="shared" si="52"/>
         <v>340.60599999999999</v>
       </c>
-      <c r="N80" s="9">
+      <c r="N80" s="5">
         <f t="shared" si="51"/>
         <v>176.64400000000001</v>
       </c>
-      <c r="O80" s="9">
+      <c r="O80" s="5">
         <f t="shared" si="51"/>
         <v>115.508</v>
       </c>
-      <c r="P80" s="9">
+      <c r="P80" s="5">
         <f t="shared" si="51"/>
         <v>88.34</v>
       </c>
-      <c r="Q80" s="9">
+      <c r="Q80" s="5">
         <f t="shared" si="51"/>
         <v>70.36</v>
       </c>
-      <c r="R80" s="9">
+      <c r="R80" s="5">
         <f t="shared" si="51"/>
         <v>70.908000000000001</v>
       </c>
-      <c r="S80" s="9">
+      <c r="S80" s="5">
         <f t="shared" si="51"/>
         <v>71.009</v>
       </c>
-      <c r="T80" s="9">
+      <c r="T80" s="5">
         <f t="shared" si="51"/>
         <v>70.733000000000004</v>
       </c>
-      <c r="U80" s="9">
+      <c r="U80" s="5">
         <f t="shared" si="51"/>
         <v>71.619</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B81">
@@ -5368,89 +5377,107 @@
       <c r="J81">
         <v>114112</v>
       </c>
-      <c r="L81" s="2" t="s">
+      <c r="L81" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M81" s="9">
+      <c r="M81" s="5">
         <f t="shared" si="52"/>
         <v>550.24400000000003</v>
       </c>
-      <c r="N81" s="9">
+      <c r="N81" s="5">
         <f t="shared" si="51"/>
         <v>286.87700000000001</v>
       </c>
-      <c r="O81" s="9">
+      <c r="O81" s="5">
         <f t="shared" si="51"/>
         <v>184.13499999999999</v>
       </c>
-      <c r="P81" s="9">
+      <c r="P81" s="5">
         <f t="shared" si="51"/>
         <v>143.13800000000001</v>
       </c>
-      <c r="Q81" s="9">
+      <c r="Q81" s="5">
         <f t="shared" si="51"/>
         <v>112.652</v>
       </c>
-      <c r="R81" s="9">
+      <c r="R81" s="5">
         <f t="shared" si="51"/>
         <v>114.973</v>
       </c>
-      <c r="S81" s="9">
+      <c r="S81" s="5">
         <f t="shared" si="51"/>
         <v>114.27200000000001</v>
       </c>
-      <c r="T81" s="9">
+      <c r="T81" s="5">
         <f t="shared" si="51"/>
         <v>113.011</v>
       </c>
-      <c r="U81" s="9">
+      <c r="U81" s="5">
         <f t="shared" si="51"/>
         <v>114.11199999999999</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="L82" s="11" t="s">
+      <c r="L82" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M82" s="12">
+      <c r="M82" s="8">
         <f xml:space="preserve"> SUM(M77:M81)/60</f>
         <v>19.083616666666668</v>
       </c>
-      <c r="N82" s="12">
+      <c r="N82" s="8">
         <f t="shared" ref="N82" si="53" xml:space="preserve"> SUM(N77:N81)/60</f>
         <v>9.9161833333333327</v>
       </c>
-      <c r="O82" s="12">
+      <c r="O82" s="8">
         <f t="shared" ref="O82" si="54" xml:space="preserve"> SUM(O77:O81)/60</f>
         <v>6.7742666666666658</v>
       </c>
-      <c r="P82" s="12">
+      <c r="P82" s="8">
         <f t="shared" ref="P82" si="55" xml:space="preserve"> SUM(P77:P81)/60</f>
         <v>5.1047666666666673</v>
       </c>
-      <c r="Q82" s="12">
+      <c r="Q82" s="8">
         <f t="shared" ref="Q82" si="56" xml:space="preserve"> SUM(Q77:Q81)/60</f>
         <v>4.1222666666666665</v>
       </c>
-      <c r="R82" s="12">
+      <c r="R82" s="8">
         <f t="shared" ref="R82" si="57" xml:space="preserve"> SUM(R77:R81)/60</f>
         <v>4.2550499999999998</v>
       </c>
-      <c r="S82" s="12">
+      <c r="S82" s="8">
         <f t="shared" ref="S82" si="58" xml:space="preserve"> SUM(S77:S81)/60</f>
         <v>4.2004000000000001</v>
       </c>
-      <c r="T82" s="12">
+      <c r="T82" s="8">
         <f t="shared" ref="T82" si="59" xml:space="preserve"> SUM(T77:T81)/60</f>
         <v>4.1424000000000003</v>
       </c>
-      <c r="U82" s="12">
+      <c r="U82" s="8">
         <f t="shared" ref="U82" si="60" xml:space="preserve"> SUM(U77:U81)/60</f>
         <v>4.1726666666666663</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="B16:J23"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="B37:J37"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="L26:U26"/>
+    <mergeCell ref="L27:U27"/>
+    <mergeCell ref="M29:U29"/>
+    <mergeCell ref="M37:U37"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="L46:U46"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="L47:U47"/>
+    <mergeCell ref="B49:J49"/>
+    <mergeCell ref="M49:U49"/>
     <mergeCell ref="B68:J68"/>
     <mergeCell ref="M68:U68"/>
     <mergeCell ref="B76:J76"/>
@@ -5461,24 +5488,6 @@
     <mergeCell ref="L65:U65"/>
     <mergeCell ref="A66:J66"/>
     <mergeCell ref="L66:U66"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="L46:U46"/>
-    <mergeCell ref="A47:J47"/>
-    <mergeCell ref="L47:U47"/>
-    <mergeCell ref="B49:J49"/>
-    <mergeCell ref="M49:U49"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="B37:J37"/>
-    <mergeCell ref="A26:J26"/>
-    <mergeCell ref="L26:U26"/>
-    <mergeCell ref="L27:U27"/>
-    <mergeCell ref="M29:U29"/>
-    <mergeCell ref="M37:U37"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="B16:J23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>